<commit_message>
Add query to create table for new geo-relevant subreddits
changes from standard table:
- Aggregate views  for 2 weeks (instead of one day)
- lower country percent threshold to 0.17 (instead of 0.40)
- Remove `active=true` filter
- Include country names
</commit_message>
<xml_diff>
--- a/reports/eda_post_lookup_table.xlsx
+++ b/reports/eda_post_lookup_table.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/david.bermejo/repos/subreddit_clustering_i18n/reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76093B45-3ED2-B14E-AD6C-694D604A21DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A93CBE7E-EE1D-8E41-B216-4DF432C5960B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8200" yWindow="6780" windowWidth="30980" windowHeight="17440" xr2:uid="{6E308B36-B0B7-0E41-AB53-CF0EF30A3608}"/>
+    <workbookView xWindow="12060" yWindow="10700" windowWidth="30980" windowHeight="17440" activeTab="1" xr2:uid="{6E308B36-B0B7-0E41-AB53-CF0EF30A3608}"/>
   </bookViews>
   <sheets>
     <sheet name="filtering verdict neutered" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>Row</t>
   </si>
@@ -43,6 +44,9 @@
   </si>
   <si>
     <t>verdict</t>
+  </si>
+  <si>
+    <t>post_id_unique_count</t>
   </si>
   <si>
     <t>null</t>
@@ -107,6 +111,15 @@
   </si>
   <si>
     <t>https://reddit.atlassian.net/wiki/spaces/DataScience/pages/2172878898/EDA+post+lookup+table</t>
+  </si>
+  <si>
+    <t>flair text</t>
+  </si>
+  <si>
+    <t>posts_with_flair_text</t>
+  </si>
+  <si>
+    <t>flair_text_unique_count</t>
   </si>
 </sst>
 </file>
@@ -516,7 +529,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAB007F8-C90C-7A4B-9999-CD9C69675BE1}">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -554,16 +567,16 @@
         <v>2</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -574,7 +587,7 @@
         <v>0</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D4" s="1">
         <v>5259970</v>
@@ -599,7 +612,7 @@
         <v>0</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D5" s="1">
         <v>56</v>
@@ -624,7 +637,7 @@
         <v>0</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D6" s="1">
         <v>12</v>
@@ -649,7 +662,7 @@
         <v>0</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D7" s="1">
         <v>520456</v>
@@ -674,7 +687,7 @@
         <v>0</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D8" s="1">
         <v>7602</v>
@@ -693,7 +706,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C10" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D10" s="5">
         <f>SUM(D4:D8)</f>
@@ -710,7 +723,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C11" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D11" s="7">
         <f>D10/$G$10</f>
@@ -723,20 +736,20 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="2:2" ht="409.6" x14ac:dyDescent="0.2">
       <c r="B17" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -749,4 +762,68 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E31932E4-3D3E-F745-B897-A644A12F8549}">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5:E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="4" width="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B2">
+        <f>5013439/7518510</f>
+        <v>0.66681283924607404</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B3">
+        <f>2505071/7518510</f>
+        <v>0.33318716075392596</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1">
+        <v>7518510</v>
+      </c>
+      <c r="D6" s="1">
+        <v>2505071</v>
+      </c>
+      <c r="E6" s="1">
+        <v>96734</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>